<commit_message>
push rank tidak perlu, push git no 1
</commit_message>
<xml_diff>
--- a/Pandas/MuhSyarifYahyaS.H/data.xlsx
+++ b/Pandas/MuhSyarifYahyaS.H/data.xlsx
@@ -461,12 +461,12 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Rata Rata</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Rank</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Rata Rata</t>
         </is>
       </c>
     </row>
@@ -489,10 +489,10 @@
         <v>81</v>
       </c>
       <c r="F2" t="n">
+        <v>80</v>
+      </c>
+      <c r="G2" t="n">
         <v>1</v>
-      </c>
-      <c r="G2" t="n">
-        <v>80</v>
       </c>
     </row>
     <row r="3">
@@ -514,10 +514,10 @@
         <v>79</v>
       </c>
       <c r="F3" t="n">
+        <v>80</v>
+      </c>
+      <c r="G3" t="n">
         <v>5</v>
-      </c>
-      <c r="G3" t="n">
-        <v>80</v>
       </c>
     </row>
     <row r="4">
@@ -539,10 +539,10 @@
         <v>80</v>
       </c>
       <c r="F4" t="n">
+        <v>80</v>
+      </c>
+      <c r="G4" t="n">
         <v>3</v>
-      </c>
-      <c r="G4" t="n">
-        <v>80</v>
       </c>
     </row>
     <row r="5">
@@ -564,10 +564,10 @@
         <v>78</v>
       </c>
       <c r="F5" t="n">
+        <v>76.7</v>
+      </c>
+      <c r="G5" t="n">
         <v>7</v>
-      </c>
-      <c r="G5" t="n">
-        <v>76.7</v>
       </c>
     </row>
     <row r="6">
@@ -589,10 +589,10 @@
         <v>68</v>
       </c>
       <c r="F6" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="G6" t="n">
         <v>10</v>
-      </c>
-      <c r="G6" t="n">
-        <v>66.7</v>
       </c>
     </row>
     <row r="7">
@@ -614,10 +614,10 @@
         <v>58</v>
       </c>
       <c r="F7" t="n">
+        <v>56.7</v>
+      </c>
+      <c r="G7" t="n">
         <v>11</v>
-      </c>
-      <c r="G7" t="n">
-        <v>56.7</v>
       </c>
     </row>
     <row r="8">
@@ -639,10 +639,10 @@
         <v>48</v>
       </c>
       <c r="F8" t="n">
+        <v>46.7</v>
+      </c>
+      <c r="G8" t="n">
         <v>12</v>
-      </c>
-      <c r="G8" t="n">
-        <v>46.7</v>
       </c>
     </row>
     <row r="9">
@@ -664,10 +664,10 @@
         <v>38</v>
       </c>
       <c r="F9" t="n">
+        <v>36.7</v>
+      </c>
+      <c r="G9" t="n">
         <v>13</v>
-      </c>
-      <c r="G9" t="n">
-        <v>36.7</v>
       </c>
     </row>
     <row r="10">
@@ -689,10 +689,10 @@
         <v>28</v>
       </c>
       <c r="F10" t="n">
+        <v>26.7</v>
+      </c>
+      <c r="G10" t="n">
         <v>14</v>
-      </c>
-      <c r="G10" t="n">
-        <v>26.7</v>
       </c>
     </row>
     <row r="11">
@@ -714,10 +714,10 @@
         <v>18</v>
       </c>
       <c r="F11" t="n">
+        <v>16.7</v>
+      </c>
+      <c r="G11" t="n">
         <v>15</v>
-      </c>
-      <c r="G11" t="n">
-        <v>16.7</v>
       </c>
     </row>
     <row r="12">
@@ -739,10 +739,10 @@
         <v>74.40000000000001</v>
       </c>
       <c r="F12" t="n">
+        <v>76</v>
+      </c>
+      <c r="G12" t="n">
         <v>9</v>
-      </c>
-      <c r="G12" t="n">
-        <v>76</v>
       </c>
     </row>
     <row r="13">
@@ -764,10 +764,10 @@
         <v>81</v>
       </c>
       <c r="F13" t="n">
+        <v>80</v>
+      </c>
+      <c r="G13" t="n">
         <v>1</v>
-      </c>
-      <c r="G13" t="n">
-        <v>80</v>
       </c>
     </row>
     <row r="14">
@@ -789,10 +789,10 @@
         <v>79</v>
       </c>
       <c r="F14" t="n">
+        <v>80</v>
+      </c>
+      <c r="G14" t="n">
         <v>5</v>
-      </c>
-      <c r="G14" t="n">
-        <v>80</v>
       </c>
     </row>
     <row r="15">
@@ -814,10 +814,10 @@
         <v>80</v>
       </c>
       <c r="F15" t="n">
+        <v>80</v>
+      </c>
+      <c r="G15" t="n">
         <v>3</v>
-      </c>
-      <c r="G15" t="n">
-        <v>80</v>
       </c>
     </row>
     <row r="16">
@@ -839,10 +839,10 @@
         <v>78</v>
       </c>
       <c r="F16" t="n">
+        <v>76.7</v>
+      </c>
+      <c r="G16" t="n">
         <v>7</v>
-      </c>
-      <c r="G16" t="n">
-        <v>76.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>